<commit_message>
se modificaron rutas de acceso de febrero, y se agregaron textos descriptivos
</commit_message>
<xml_diff>
--- a/Data/2023/2. Febrero2023/Registro_de_operaciones_Roboforex_Febrero2023.xlsx
+++ b/Data/2023/2. Febrero2023/Registro_de_operaciones_Roboforex_Febrero2023.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\samue\Documents\QuantResearch\Recolección de datos\7. Febrero2023\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Coding\QuantCo_Streamlit\Data\2023\2. Febrero2023\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C763460-A15B-477A-AA65-C4ECE13B754A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC0C4F84-F219-4629-8EE9-8929458BAF3F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Report" sheetId="1" r:id="rId1"/>
@@ -780,24 +780,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I113"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A73" workbookViewId="0">
-      <selection activeCell="K85" sqref="K85"/>
+    <sheetView tabSelected="1" topLeftCell="A82" workbookViewId="0">
+      <selection activeCell="N113" sqref="N113"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="17.69921875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.19921875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="4.8984375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.75" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.25" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="4.875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="8.5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.8984375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="5.69921875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.796875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="5.75" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.75" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="6.5" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="8.3984375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="8.375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" s="5" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>124</v>
       </c>
@@ -826,7 +826,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -857,7 +857,7 @@
         <v>10846.869999999999</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -888,7 +888,7 @@
         <v>10848.72</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>9</v>
       </c>
@@ -919,7 +919,7 @@
         <v>10850.63</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>10</v>
       </c>
@@ -950,7 +950,7 @@
         <v>10852.57</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>11</v>
       </c>
@@ -981,7 +981,7 @@
         <v>10845.46</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>13</v>
       </c>
@@ -1012,7 +1012,7 @@
         <v>10840.56</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>14</v>
       </c>
@@ -1043,7 +1043,7 @@
         <v>10841.59</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>15</v>
       </c>
@@ -1074,7 +1074,7 @@
         <v>10843.44</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>16</v>
       </c>
@@ -1105,7 +1105,7 @@
         <v>10845.25</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>17</v>
       </c>
@@ -1136,7 +1136,7 @@
         <v>10847.18</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>18</v>
       </c>
@@ -1167,7 +1167,7 @@
         <v>10849.09</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>19</v>
       </c>
@@ -1198,7 +1198,7 @@
         <v>10850.880000000001</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>20</v>
       </c>
@@ -1229,7 +1229,7 @@
         <v>10850.570000000002</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>21</v>
       </c>
@@ -1260,7 +1260,7 @@
         <v>10855.87</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>22</v>
       </c>
@@ -1291,7 +1291,7 @@
         <v>10857.800000000001</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>23</v>
       </c>
@@ -1322,7 +1322,7 @@
         <v>10859.710000000001</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>24</v>
       </c>
@@ -1353,7 +1353,7 @@
         <v>10861.560000000001</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>25</v>
       </c>
@@ -1384,7 +1384,7 @@
         <v>10863.45</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>26</v>
       </c>
@@ -1415,7 +1415,7 @@
         <v>10865.36</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>27</v>
       </c>
@@ -1446,7 +1446,7 @@
         <v>10851.650000000001</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>28</v>
       </c>
@@ -1477,7 +1477,7 @@
         <v>10839.580000000002</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>29</v>
       </c>
@@ -1508,7 +1508,7 @@
         <v>10839.29</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>30</v>
       </c>
@@ -1539,7 +1539,7 @@
         <v>10849.330000000002</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>31</v>
       </c>
@@ -1570,7 +1570,7 @@
         <v>10864.590000000002</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>32</v>
       </c>
@@ -1601,7 +1601,7 @@
         <v>10878.640000000001</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>33</v>
       </c>
@@ -1632,7 +1632,7 @@
         <v>10876.03</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>34</v>
       </c>
@@ -1663,7 +1663,7 @@
         <v>10877.67</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>35</v>
       </c>
@@ -1694,7 +1694,7 @@
         <v>10887.18</v>
       </c>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>36</v>
       </c>
@@ -1725,7 +1725,7 @@
         <v>10889.130000000001</v>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>37</v>
       </c>
@@ -1756,7 +1756,7 @@
         <v>10891.000000000002</v>
       </c>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>38</v>
       </c>
@@ -1787,7 +1787,7 @@
         <v>10882.770000000002</v>
       </c>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>39</v>
       </c>
@@ -1818,7 +1818,7 @@
         <v>10882.100000000002</v>
       </c>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>40</v>
       </c>
@@ -1849,7 +1849,7 @@
         <v>10889.650000000001</v>
       </c>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>41</v>
       </c>
@@ -1880,7 +1880,7 @@
         <v>10898.730000000001</v>
       </c>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>42</v>
       </c>
@@ -1911,7 +1911,7 @@
         <v>10900.560000000001</v>
       </c>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>43</v>
       </c>
@@ -1942,7 +1942,7 @@
         <v>10902.510000000002</v>
       </c>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>44</v>
       </c>
@@ -1973,7 +1973,7 @@
         <v>10902.180000000002</v>
       </c>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>45</v>
       </c>
@@ -2004,7 +2004,7 @@
         <v>10907.240000000002</v>
       </c>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>46</v>
       </c>
@@ -2035,7 +2035,7 @@
         <v>10909.170000000002</v>
       </c>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>47</v>
       </c>
@@ -2066,7 +2066,7 @@
         <v>10911.000000000002</v>
       </c>
     </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>48</v>
       </c>
@@ -2097,7 +2097,7 @@
         <v>10912.870000000003</v>
       </c>
     </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>49</v>
       </c>
@@ -2128,7 +2128,7 @@
         <v>10914.840000000002</v>
       </c>
     </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>50</v>
       </c>
@@ -2159,7 +2159,7 @@
         <v>10914.430000000002</v>
       </c>
     </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>51</v>
       </c>
@@ -2190,7 +2190,7 @@
         <v>10919.640000000001</v>
       </c>
     </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>52</v>
       </c>
@@ -2221,7 +2221,7 @@
         <v>10919.19</v>
       </c>
     </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>53</v>
       </c>
@@ -2252,7 +2252,7 @@
         <v>10924.16</v>
       </c>
     </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>54</v>
       </c>
@@ -2283,7 +2283,7 @@
         <v>10910.61</v>
       </c>
     </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>55</v>
       </c>
@@ -2314,7 +2314,7 @@
         <v>10894.37</v>
       </c>
     </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>56</v>
       </c>
@@ -2345,7 +2345,7 @@
         <v>10874.240000000002</v>
       </c>
     </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>57</v>
       </c>
@@ -2376,7 +2376,7 @@
         <v>10865.030000000002</v>
       </c>
     </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>58</v>
       </c>
@@ -2407,7 +2407,7 @@
         <v>10868.210000000003</v>
       </c>
     </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>59</v>
       </c>
@@ -2438,7 +2438,7 @@
         <v>10882.150000000003</v>
       </c>
     </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>60</v>
       </c>
@@ -2469,7 +2469,7 @@
         <v>10884.850000000004</v>
       </c>
     </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>61</v>
       </c>
@@ -2500,7 +2500,7 @@
         <v>10908.680000000004</v>
       </c>
     </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>62</v>
       </c>
@@ -2531,7 +2531,7 @@
         <v>10932.050000000005</v>
       </c>
     </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>63</v>
       </c>
@@ -2562,7 +2562,7 @@
         <v>10931.820000000005</v>
       </c>
     </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>64</v>
       </c>
@@ -2593,7 +2593,7 @@
         <v>10937.120000000004</v>
       </c>
     </row>
-    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>65</v>
       </c>
@@ -2624,7 +2624,7 @@
         <v>10937.150000000005</v>
       </c>
     </row>
-    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>66</v>
       </c>
@@ -2655,7 +2655,7 @@
         <v>10942.960000000005</v>
       </c>
     </row>
-    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>67</v>
       </c>
@@ -2686,7 +2686,7 @@
         <v>10944.870000000004</v>
       </c>
     </row>
-    <row r="62" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>68</v>
       </c>
@@ -2717,7 +2717,7 @@
         <v>10946.660000000005</v>
       </c>
     </row>
-    <row r="63" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>69</v>
       </c>
@@ -2748,7 +2748,7 @@
         <v>10948.550000000005</v>
       </c>
     </row>
-    <row r="64" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>70</v>
       </c>
@@ -2779,7 +2779,7 @@
         <v>10950.420000000006</v>
       </c>
     </row>
-    <row r="65" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>71</v>
       </c>
@@ -2810,7 +2810,7 @@
         <v>10952.310000000005</v>
       </c>
     </row>
-    <row r="66" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>72</v>
       </c>
@@ -2841,7 +2841,7 @@
         <v>10954.200000000004</v>
       </c>
     </row>
-    <row r="67" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>73</v>
       </c>
@@ -2872,7 +2872,7 @@
         <v>10956.030000000004</v>
       </c>
     </row>
-    <row r="68" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>74</v>
       </c>
@@ -2903,7 +2903,7 @@
         <v>10954.560000000005</v>
       </c>
     </row>
-    <row r="69" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>75</v>
       </c>
@@ -2934,7 +2934,7 @@
         <v>10955.870000000004</v>
       </c>
     </row>
-    <row r="70" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>76</v>
       </c>
@@ -2965,7 +2965,7 @@
         <v>10961.860000000004</v>
       </c>
     </row>
-    <row r="71" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>77</v>
       </c>
@@ -2996,7 +2996,7 @@
         <v>10961.530000000004</v>
       </c>
     </row>
-    <row r="72" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>78</v>
       </c>
@@ -3027,7 +3027,7 @@
         <v>10966.410000000003</v>
       </c>
     </row>
-    <row r="73" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>79</v>
       </c>
@@ -3058,7 +3058,7 @@
         <v>10968.260000000004</v>
       </c>
     </row>
-    <row r="74" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>80</v>
       </c>
@@ -3089,7 +3089,7 @@
         <v>10970.150000000003</v>
       </c>
     </row>
-    <row r="75" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>81</v>
       </c>
@@ -3120,7 +3120,7 @@
         <v>10971.960000000003</v>
       </c>
     </row>
-    <row r="76" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>82</v>
       </c>
@@ -3151,7 +3151,7 @@
         <v>10973.930000000002</v>
       </c>
     </row>
-    <row r="77" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>83</v>
       </c>
@@ -3182,7 +3182,7 @@
         <v>10975.800000000003</v>
       </c>
     </row>
-    <row r="78" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>84</v>
       </c>
@@ -3213,7 +3213,7 @@
         <v>10977.590000000004</v>
       </c>
     </row>
-    <row r="79" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>85</v>
       </c>
@@ -3244,7 +3244,7 @@
         <v>10977.340000000004</v>
       </c>
     </row>
-    <row r="80" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>86</v>
       </c>
@@ -3275,7 +3275,7 @@
         <v>10982.700000000004</v>
       </c>
     </row>
-    <row r="81" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>87</v>
       </c>
@@ -3306,7 +3306,7 @@
         <v>10982.210000000005</v>
       </c>
     </row>
-    <row r="82" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>88</v>
       </c>
@@ -3337,7 +3337,7 @@
         <v>10987.180000000004</v>
       </c>
     </row>
-    <row r="83" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>89</v>
       </c>
@@ -3368,7 +3368,7 @@
         <v>10988.970000000005</v>
       </c>
     </row>
-    <row r="84" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>90</v>
       </c>
@@ -3399,7 +3399,7 @@
         <v>10990.860000000004</v>
       </c>
     </row>
-    <row r="85" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>91</v>
       </c>
@@ -3430,7 +3430,7 @@
         <v>10990.390000000005</v>
       </c>
     </row>
-    <row r="86" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>92</v>
       </c>
@@ -3461,7 +3461,7 @@
         <v>10995.570000000005</v>
       </c>
     </row>
-    <row r="87" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>93</v>
       </c>
@@ -3492,7 +3492,7 @@
         <v>10997.480000000005</v>
       </c>
     </row>
-    <row r="88" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>94</v>
       </c>
@@ -3523,7 +3523,7 @@
         <v>10999.250000000005</v>
       </c>
     </row>
-    <row r="89" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>95</v>
       </c>
@@ -3554,7 +3554,7 @@
         <v>11001.120000000006</v>
       </c>
     </row>
-    <row r="90" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>96</v>
       </c>
@@ -3585,7 +3585,7 @@
         <v>11000.630000000006</v>
       </c>
     </row>
-    <row r="91" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>97</v>
       </c>
@@ -3616,7 +3616,7 @@
         <v>11005.570000000007</v>
       </c>
     </row>
-    <row r="92" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>98</v>
       </c>
@@ -3647,7 +3647,7 @@
         <v>11007.360000000008</v>
       </c>
     </row>
-    <row r="93" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>99</v>
       </c>
@@ -3678,7 +3678,7 @@
         <v>11007.190000000008</v>
       </c>
     </row>
-    <row r="94" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>100</v>
       </c>
@@ -3709,7 +3709,7 @@
         <v>11012.790000000008</v>
       </c>
     </row>
-    <row r="95" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>101</v>
       </c>
@@ -3740,7 +3740,7 @@
         <v>11014.710000000008</v>
       </c>
     </row>
-    <row r="96" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>102</v>
       </c>
@@ -3771,7 +3771,7 @@
         <v>11014.230000000009</v>
       </c>
     </row>
-    <row r="97" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>103</v>
       </c>
@@ -3802,7 +3802,7 @@
         <v>11019.200000000008</v>
       </c>
     </row>
-    <row r="98" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>104</v>
       </c>
@@ -3833,7 +3833,7 @@
         <v>11021.100000000008</v>
       </c>
     </row>
-    <row r="99" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>105</v>
       </c>
@@ -3864,7 +3864,7 @@
         <v>11023.000000000007</v>
       </c>
     </row>
-    <row r="100" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>106</v>
       </c>
@@ -3895,7 +3895,7 @@
         <v>11024.880000000006</v>
       </c>
     </row>
-    <row r="101" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
         <v>107</v>
       </c>
@@ -3926,7 +3926,7 @@
         <v>11012.340000000006</v>
       </c>
     </row>
-    <row r="102" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
         <v>108</v>
       </c>
@@ -3957,7 +3957,7 @@
         <v>10993.370000000006</v>
       </c>
     </row>
-    <row r="103" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
         <v>109</v>
       </c>
@@ -3988,7 +3988,7 @@
         <v>10975.960000000006</v>
       </c>
     </row>
-    <row r="104" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
         <v>110</v>
       </c>
@@ -4019,7 +4019,7 @@
         <v>10974.750000000007</v>
       </c>
     </row>
-    <row r="105" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
         <v>111</v>
       </c>
@@ -4050,7 +4050,7 @@
         <v>10987.850000000008</v>
       </c>
     </row>
-    <row r="106" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
         <v>112</v>
       </c>
@@ -4081,7 +4081,7 @@
         <v>11001.430000000008</v>
       </c>
     </row>
-    <row r="107" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
         <v>113</v>
       </c>
@@ -4112,7 +4112,7 @@
         <v>11020.600000000008</v>
       </c>
     </row>
-    <row r="108" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
         <v>114</v>
       </c>
@@ -4143,7 +4143,7 @@
         <v>11038.830000000007</v>
       </c>
     </row>
-    <row r="109" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
         <v>115</v>
       </c>
@@ -4174,7 +4174,7 @@
         <v>11040.770000000008</v>
       </c>
     </row>
-    <row r="110" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
         <v>116</v>
       </c>
@@ -4205,7 +4205,7 @@
         <v>11042.630000000008</v>
       </c>
     </row>
-    <row r="111" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
         <v>117</v>
       </c>
@@ -4233,7 +4233,7 @@
         <v>11050.770000000008</v>
       </c>
     </row>
-    <row r="112" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
         <v>117</v>
       </c>
@@ -4261,7 +4261,7 @@
         <v>11052.390000000009</v>
       </c>
     </row>
-    <row r="113" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
         <v>119</v>
       </c>

</xml_diff>